<commit_message>
invastigate imgs of event page
</commit_message>
<xml_diff>
--- a/เอกสารPnP/Snack box.xlsx
+++ b/เอกสารPnP/Snack box.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pree_site\Puff n Pie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pree_site\Puff n Pie\เอกสารPnP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Snack Boxes" sheetId="11" r:id="rId1"/>
@@ -710,9 +710,6 @@
     <t>Email : ongroundsales@thaiairways.com</t>
   </si>
   <si>
-    <t>Email : puffandpiie.admin@thaiairways.com</t>
-  </si>
-  <si>
     <t>ฝ่ายครัวการบินไทย ดอนเมือง
 เลขที่ 171/1 แขวงสนามบิน ดอนเมือง กรุงเทพฯ 10210</t>
   </si>
@@ -727,6 +724,9 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>Email : puffandpie.admin@thaiairways.com</t>
   </si>
 </sst>
 </file>
@@ -1460,6 +1460,75 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1502,76 +1571,7 @@
     <xf numFmtId="49" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1624,7 +1624,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65AF30C8-EFCA-4E78-A3A0-5C37C6F1A49D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65AF30C8-EFCA-4E78-A3A0-5C37C6F1A49D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1667,7 +1667,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CFD7CA94-CEE2-49B7-985B-B396DD7928AF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFD7CA94-CEE2-49B7-985B-B396DD7928AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1711,7 +1711,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E207F21A-0A84-4ABB-893A-B6B3A2D25235}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E207F21A-0A84-4ABB-893A-B6B3A2D25235}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1755,7 +1755,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F96B9F94-AAF0-4403-A80F-0A238AA0EA4C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F96B9F94-AAF0-4403-A80F-0A238AA0EA4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1799,7 +1799,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7DBD78D4-BB90-4E91-95F5-FA26DF570217}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DBD78D4-BB90-4E91-95F5-FA26DF570217}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1843,7 +1843,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F8A907E-0FEC-4F8A-BE51-085894930FC4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F8A907E-0FEC-4F8A-BE51-085894930FC4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1887,7 +1887,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B80D9125-1482-470A-AE33-38258B12AFBC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B80D9125-1482-470A-AE33-38258B12AFBC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1931,7 +1931,7 @@
         <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F019455D-0598-4F2B-95DE-A6DEEB27A2C0}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F019455D-0598-4F2B-95DE-A6DEEB27A2C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1975,7 +1975,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{56C5B69F-AEEC-4630-8FFE-9DAA1FAA2159}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56C5B69F-AEEC-4630-8FFE-9DAA1FAA2159}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2019,7 +2019,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1D88B59-65D5-41A4-84C3-9801C6221F5D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1D88B59-65D5-41A4-84C3-9801C6221F5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2063,7 +2063,7 @@
         <xdr:cNvPr id="19" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AFDA0967-B11A-4CA1-8DC3-33C92B746946}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFDA0967-B11A-4CA1-8DC3-33C92B746946}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2107,7 +2107,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{19A7F5D0-3C99-47ED-A540-DE742976C9F5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19A7F5D0-3C99-47ED-A540-DE742976C9F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2151,7 +2151,7 @@
         <xdr:cNvPr id="21" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{417D9800-1E0F-47D0-A88B-69FD0F8392B4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{417D9800-1E0F-47D0-A88B-69FD0F8392B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2195,7 +2195,7 @@
         <xdr:cNvPr id="22" name="Picture 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79AB404D-B5DA-4387-BA90-554480C4D824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79AB404D-B5DA-4387-BA90-554480C4D824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2239,7 +2239,7 @@
         <xdr:cNvPr id="23" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53A037CB-DD3B-46C6-8AB1-3C4D3DF76C93}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53A037CB-DD3B-46C6-8AB1-3C4D3DF76C93}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2283,7 +2283,7 @@
         <xdr:cNvPr id="25" name="Picture 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{38A667B3-57B9-4D1E-91AD-FE636001749D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38A667B3-57B9-4D1E-91AD-FE636001749D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2327,7 +2327,7 @@
         <xdr:cNvPr id="26" name="Picture 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4A93623E-BBA4-4167-8ABB-016CCB37B91A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A93623E-BBA4-4167-8ABB-016CCB37B91A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2371,7 +2371,7 @@
         <xdr:cNvPr id="28" name="Picture 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CC609169-F0DE-49AA-A491-0C622653ECAA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC609169-F0DE-49AA-A491-0C622653ECAA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2415,7 +2415,7 @@
         <xdr:cNvPr id="29" name="Picture 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2D766E38-0BFD-44A7-86CF-2D114E7E6BC2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D766E38-0BFD-44A7-86CF-2D114E7E6BC2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2459,7 +2459,7 @@
         <xdr:cNvPr id="30" name="Picture 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{71FA2900-21A2-4F52-91BF-FC7182DF3988}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71FA2900-21A2-4F52-91BF-FC7182DF3988}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2503,7 +2503,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{27D7644C-6FC2-45BA-BE6B-3DDF6BA6833F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27D7644C-6FC2-45BA-BE6B-3DDF6BA6833F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2547,7 +2547,7 @@
         <xdr:cNvPr id="32" name="Picture 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6713EF2E-57D4-452E-9CC6-6F9B3E3F422E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6713EF2E-57D4-452E-9CC6-6F9B3E3F422E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2591,7 +2591,7 @@
         <xdr:cNvPr id="33" name="Picture 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{05EF6FAC-3E41-4669-9CB6-6360A33F36A4}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05EF6FAC-3E41-4669-9CB6-6360A33F36A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2635,7 +2635,7 @@
         <xdr:cNvPr id="34" name="Picture 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{75CB5E3B-BAF8-4C09-A251-19877F98AD63}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75CB5E3B-BAF8-4C09-A251-19877F98AD63}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2679,7 +2679,7 @@
         <xdr:cNvPr id="35" name="Picture 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{45719B70-55CD-4D41-B672-01FC6D9D96FB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45719B70-55CD-4D41-B672-01FC6D9D96FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2723,7 +2723,7 @@
         <xdr:cNvPr id="36" name="Picture 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{96ECC012-BF1D-4EAA-976F-22F7790A8D84}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96ECC012-BF1D-4EAA-976F-22F7790A8D84}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2767,7 +2767,7 @@
         <xdr:cNvPr id="37" name="Picture 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4341422F-F9C0-433C-BBAC-8A43B5C3BF99}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4341422F-F9C0-433C-BBAC-8A43B5C3BF99}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2811,7 +2811,7 @@
         <xdr:cNvPr id="38" name="Picture 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C2D9A36-E54F-4700-B246-E1D05D3516D6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C2D9A36-E54F-4700-B246-E1D05D3516D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2855,7 +2855,7 @@
         <xdr:cNvPr id="39" name="Picture 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C3CF150A-7E38-4FDE-AD5C-3B91AF8A31AB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3CF150A-7E38-4FDE-AD5C-3B91AF8A31AB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2899,7 +2899,7 @@
         <xdr:cNvPr id="40" name="Picture 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{128D8B6F-F84A-44BD-ADEE-1707FE12B0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{128D8B6F-F84A-44BD-ADEE-1707FE12B0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2943,7 +2943,7 @@
         <xdr:cNvPr id="41" name="Picture 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3BA7FAAB-030D-43FC-9321-391DDE7C0BE3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BA7FAAB-030D-43FC-9321-391DDE7C0BE3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2987,7 +2987,7 @@
         <xdr:cNvPr id="42" name="Picture 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A8C30939-8D61-4B1B-829B-62A78B5F06F5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C30939-8D61-4B1B-829B-62A78B5F06F5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3031,7 +3031,7 @@
         <xdr:cNvPr id="43" name="Picture 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{25CFF077-F01D-47BE-8947-4B67479FEEB8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25CFF077-F01D-47BE-8947-4B67479FEEB8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3075,7 +3075,7 @@
         <xdr:cNvPr id="44" name="Picture 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A27BA787-D152-4A1E-8AE9-A5AB7C2714BB}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A27BA787-D152-4A1E-8AE9-A5AB7C2714BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3119,7 +3119,7 @@
         <xdr:cNvPr id="45" name="Picture 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{511348A8-5E23-4AFF-B9CA-8C949D65E4DF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{511348A8-5E23-4AFF-B9CA-8C949D65E4DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3163,7 +3163,7 @@
         <xdr:cNvPr id="46" name="Picture 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{260F91E2-03F6-46B6-B8E7-02D1BED2279D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{260F91E2-03F6-46B6-B8E7-02D1BED2279D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3207,7 +3207,7 @@
         <xdr:cNvPr id="47" name="Picture 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{575866B7-5E46-4166-8D69-0B8193558B8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{575866B7-5E46-4166-8D69-0B8193558B8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3251,7 +3251,7 @@
         <xdr:cNvPr id="48" name="Picture 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DD7864E7-EDAF-4B02-B62C-C9CFD1AAD3B1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD7864E7-EDAF-4B02-B62C-C9CFD1AAD3B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3295,7 +3295,7 @@
         <xdr:cNvPr id="49" name="Picture 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FECED7BF-2D4B-41A5-9278-D05402016725}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FECED7BF-2D4B-41A5-9278-D05402016725}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3339,7 +3339,7 @@
         <xdr:cNvPr id="50" name="Picture 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D3F83E5-5005-4E98-BAB6-7E416599D2B2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D3F83E5-5005-4E98-BAB6-7E416599D2B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3383,7 +3383,7 @@
         <xdr:cNvPr id="51" name="Picture 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73DBF665-E698-42FA-8DF2-3BF09CA2628E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73DBF665-E698-42FA-8DF2-3BF09CA2628E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3427,7 +3427,7 @@
         <xdr:cNvPr id="52" name="Picture 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4F41D149-C401-413A-8F34-B8ABBE55BE34}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F41D149-C401-413A-8F34-B8ABBE55BE34}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3471,7 +3471,7 @@
         <xdr:cNvPr id="53" name="Picture 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DA367FD5-1019-4979-A408-55D22ACB99F8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA367FD5-1019-4979-A408-55D22ACB99F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3515,7 +3515,7 @@
         <xdr:cNvPr id="54" name="Picture 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5239E47-C06F-410E-A9C2-8C877FEA3F87}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5239E47-C06F-410E-A9C2-8C877FEA3F87}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3559,7 +3559,7 @@
         <xdr:cNvPr id="55" name="Picture 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E8EC99AE-28E1-4953-ABD6-3FDA87D86D1A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8EC99AE-28E1-4953-ABD6-3FDA87D86D1A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3603,7 +3603,7 @@
         <xdr:cNvPr id="56" name="Picture 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F066E2D-677D-4246-A80E-02713FEF68A1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F066E2D-677D-4246-A80E-02713FEF68A1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3647,7 +3647,7 @@
         <xdr:cNvPr id="58" name="Picture 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{127329DC-AB47-46A0-ADF8-168E28AA78C3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{127329DC-AB47-46A0-ADF8-168E28AA78C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3691,7 +3691,7 @@
         <xdr:cNvPr id="59" name="Picture 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D21626AF-C621-465C-B8E2-EAEB7BB7EFF2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D21626AF-C621-465C-B8E2-EAEB7BB7EFF2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3735,7 +3735,7 @@
         <xdr:cNvPr id="61" name="Picture 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{84D44AD5-BB94-4E53-869D-304F910EA886}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84D44AD5-BB94-4E53-869D-304F910EA886}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3784,7 +3784,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5835D521-21FF-47FC-BF03-C842912ADC0F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5835D521-21FF-47FC-BF03-C842912ADC0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3828,7 +3828,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{05596DC5-896D-4DF4-A380-26178A0649D7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05596DC5-896D-4DF4-A380-26178A0649D7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3872,7 +3872,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{781A2969-EB55-4675-8978-E1800D7319F9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{781A2969-EB55-4675-8978-E1800D7319F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3916,7 +3916,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{673F6A9E-B163-42CE-A644-8F1E6EAAA06E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{673F6A9E-B163-42CE-A644-8F1E6EAAA06E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4266,16 +4266,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="84"/>
     </row>
     <row r="2" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -4284,18 +4284,18 @@
       <c r="B2" s="44">
         <v>55</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="64" t="s">
+      <c r="D2" s="85"/>
+      <c r="E2" s="87" t="s">
         <v>81</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="62"/>
-      <c r="H2" s="66"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="89"/>
     </row>
     <row r="3" spans="1:12" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
@@ -4304,30 +4304,30 @@
       <c r="B3" s="42">
         <v>65</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="63"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="63" t="s">
+      <c r="D3" s="86"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="67"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="90"/>
     </row>
     <row r="4" spans="1:12" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="79"/>
     </row>
     <row r="5" spans="1:12" s="18" customFormat="1" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
@@ -4354,25 +4354,25 @@
       <c r="H5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
     </row>
     <row r="6" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="B6" s="91">
+      <c r="B6" s="60">
         <v>1</v>
       </c>
-      <c r="C6" s="85"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="86">
+      <c r="E6" s="62">
         <v>15</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -4399,12 +4399,12 @@
     </row>
     <row r="7" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="71"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="75"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
       <c r="D7" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="79"/>
+      <c r="E7" s="56"/>
       <c r="F7" s="5" t="s">
         <v>34</v>
       </c>
@@ -4431,14 +4431,14 @@
       <c r="A8" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="88">
+      <c r="B8" s="54">
         <v>2</v>
       </c>
-      <c r="C8" s="75"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="79">
+      <c r="E8" s="56">
         <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -4465,12 +4465,12 @@
     </row>
     <row r="9" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="71"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="75"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="79"/>
+      <c r="E9" s="56"/>
       <c r="F9" s="5" t="s">
         <v>176</v>
       </c>
@@ -4497,14 +4497,14 @@
       <c r="A10" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="88">
+      <c r="B10" s="54">
         <v>3</v>
       </c>
-      <c r="C10" s="75"/>
+      <c r="C10" s="55"/>
       <c r="D10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="79">
+      <c r="E10" s="56">
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -4531,12 +4531,12 @@
     </row>
     <row r="11" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="71"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="75"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="79"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="5" t="s">
         <v>36</v>
       </c>
@@ -4563,14 +4563,14 @@
       <c r="A12" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="88">
+      <c r="B12" s="54">
         <v>4</v>
       </c>
-      <c r="C12" s="75"/>
+      <c r="C12" s="55"/>
       <c r="D12" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="79">
+      <c r="E12" s="56">
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -4597,12 +4597,12 @@
     </row>
     <row r="13" spans="1:12" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="72"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="80"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="58"/>
       <c r="D13" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="81"/>
+      <c r="E13" s="59"/>
       <c r="F13" s="9" t="s">
         <v>178</v>
       </c>
@@ -4629,14 +4629,14 @@
       <c r="A14" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="82">
+      <c r="B14" s="64">
         <v>5</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="83">
+      <c r="E14" s="65">
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -4663,12 +4663,12 @@
     </row>
     <row r="15" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="71"/>
-      <c r="B15" s="75"/>
-      <c r="C15" s="75"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="79"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="5" t="s">
         <v>180</v>
       </c>
@@ -4695,14 +4695,14 @@
       <c r="A16" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="75">
+      <c r="B16" s="55">
         <v>6</v>
       </c>
-      <c r="C16" s="75"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="E16" s="79">
+      <c r="E16" s="56">
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -4729,12 +4729,12 @@
     </row>
     <row r="17" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="71"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="55"/>
       <c r="D17" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="79"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="3" t="s">
         <v>181</v>
       </c>
@@ -4761,14 +4761,14 @@
       <c r="A18" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="88">
+      <c r="B18" s="54">
         <v>7</v>
       </c>
-      <c r="C18" s="75"/>
+      <c r="C18" s="55"/>
       <c r="D18" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="79">
+      <c r="E18" s="56">
         <v>15</v>
       </c>
       <c r="F18" s="5" t="s">
@@ -4795,12 +4795,12 @@
     </row>
     <row r="19" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="71"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="75"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="79"/>
+      <c r="E19" s="56"/>
       <c r="F19" s="5" t="s">
         <v>60</v>
       </c>
@@ -4827,14 +4827,14 @@
       <c r="A20" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="88">
+      <c r="B20" s="54">
         <v>8</v>
       </c>
-      <c r="C20" s="75"/>
+      <c r="C20" s="55"/>
       <c r="D20" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="76"/>
+      <c r="E20" s="63"/>
       <c r="F20" s="31"/>
       <c r="G20" s="5" t="s">
         <v>27</v>
@@ -4857,12 +4857,12 @@
     </row>
     <row r="21" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="71"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="75"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="76"/>
+      <c r="E21" s="63"/>
       <c r="F21" s="31"/>
       <c r="G21" s="5" t="s">
         <v>26</v>
@@ -4887,14 +4887,14 @@
       <c r="A22" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="88" t="s">
-        <v>229</v>
-      </c>
-      <c r="C22" s="75"/>
+      <c r="B22" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="C22" s="55"/>
       <c r="D22" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="E22" s="79">
+      <c r="E22" s="56">
         <v>15</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -4921,12 +4921,12 @@
     </row>
     <row r="23" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="71"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="75"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="55"/>
       <c r="D23" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="E23" s="79"/>
+      <c r="E23" s="56"/>
       <c r="F23" s="3" t="s">
         <v>181</v>
       </c>
@@ -4947,14 +4947,14 @@
       <c r="A24" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="88">
+      <c r="B24" s="54">
         <v>10</v>
       </c>
-      <c r="C24" s="75"/>
+      <c r="C24" s="55"/>
       <c r="D24" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="E24" s="79">
+      <c r="E24" s="56">
         <v>15</v>
       </c>
       <c r="F24" s="5" t="s">
@@ -4975,12 +4975,12 @@
     </row>
     <row r="25" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="71"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="75"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
       <c r="D25" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="E25" s="79"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="3" t="s">
         <v>181</v>
       </c>
@@ -5001,14 +5001,14 @@
       <c r="A26" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="75">
+      <c r="B26" s="55">
         <v>11</v>
       </c>
-      <c r="C26" s="75"/>
+      <c r="C26" s="55"/>
       <c r="D26" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="E26" s="79">
+      <c r="E26" s="56">
         <v>15</v>
       </c>
       <c r="F26" s="5" t="s">
@@ -5029,12 +5029,12 @@
     </row>
     <row r="27" spans="1:12" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="72"/>
-      <c r="B27" s="80"/>
-      <c r="C27" s="80"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="58"/>
       <c r="D27" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="81"/>
+      <c r="E27" s="59"/>
       <c r="F27" s="9" t="s">
         <v>183</v>
       </c>
@@ -5055,14 +5055,14 @@
       <c r="A28" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="B28" s="90">
+      <c r="B28" s="66">
         <v>12</v>
       </c>
-      <c r="C28" s="82"/>
+      <c r="C28" s="64"/>
       <c r="D28" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="83">
+      <c r="E28" s="65">
         <v>12</v>
       </c>
       <c r="F28" s="2" t="s">
@@ -5083,12 +5083,12 @@
     </row>
     <row r="29" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="71"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="75"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
       <c r="D29" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="79"/>
+      <c r="E29" s="56"/>
       <c r="F29" s="5" t="s">
         <v>48</v>
       </c>
@@ -5109,14 +5109,14 @@
       <c r="A30" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="88">
+      <c r="B30" s="54">
         <v>13</v>
       </c>
-      <c r="C30" s="75"/>
+      <c r="C30" s="55"/>
       <c r="D30" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="79">
+      <c r="E30" s="56">
         <v>12</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -5131,12 +5131,12 @@
     </row>
     <row r="31" spans="1:12" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="71"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="75"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="55"/>
       <c r="D31" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E31" s="79"/>
+      <c r="E31" s="56"/>
       <c r="F31" s="5" t="s">
         <v>47</v>
       </c>
@@ -5151,14 +5151,14 @@
       <c r="A32" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="75">
+      <c r="B32" s="55">
         <v>14</v>
       </c>
-      <c r="C32" s="75"/>
+      <c r="C32" s="55"/>
       <c r="D32" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="79">
+      <c r="E32" s="56">
         <v>12</v>
       </c>
       <c r="F32" s="5" t="s">
@@ -5173,12 +5173,12 @@
     </row>
     <row r="33" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="71"/>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
       <c r="D33" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E33" s="79"/>
+      <c r="E33" s="56"/>
       <c r="F33" s="5" t="s">
         <v>48</v>
       </c>
@@ -5193,14 +5193,14 @@
       <c r="A34" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="88">
+      <c r="B34" s="54">
         <v>15</v>
       </c>
-      <c r="C34" s="75"/>
+      <c r="C34" s="55"/>
       <c r="D34" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="79">
+      <c r="E34" s="56">
         <v>12</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -5215,12 +5215,12 @@
     </row>
     <row r="35" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="71"/>
-      <c r="B35" s="88"/>
-      <c r="C35" s="75"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="55"/>
       <c r="D35" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="79"/>
+      <c r="E35" s="56"/>
       <c r="F35" s="5" t="s">
         <v>49</v>
       </c>
@@ -5235,14 +5235,14 @@
       <c r="A36" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="75">
+      <c r="B36" s="55">
         <v>16</v>
       </c>
-      <c r="C36" s="75"/>
+      <c r="C36" s="55"/>
       <c r="D36" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="79">
+      <c r="E36" s="56">
         <v>12</v>
       </c>
       <c r="F36" s="5" t="s">
@@ -5257,12 +5257,12 @@
     </row>
     <row r="37" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="71"/>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="55"/>
       <c r="D37" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="79"/>
+      <c r="E37" s="56"/>
       <c r="F37" s="5" t="s">
         <v>57</v>
       </c>
@@ -5277,14 +5277,14 @@
       <c r="A38" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="88" t="s">
-        <v>228</v>
-      </c>
-      <c r="C38" s="75"/>
+      <c r="B38" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="C38" s="55"/>
       <c r="D38" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="E38" s="79">
+      <c r="E38" s="56">
         <v>12</v>
       </c>
       <c r="F38" s="5" t="s">
@@ -5299,12 +5299,12 @@
     </row>
     <row r="39" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="71"/>
-      <c r="B39" s="88"/>
-      <c r="C39" s="75"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="55"/>
       <c r="D39" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="E39" s="79"/>
+      <c r="E39" s="56"/>
       <c r="F39" s="5" t="s">
         <v>185</v>
       </c>
@@ -5319,14 +5319,14 @@
       <c r="A40" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="75">
+      <c r="B40" s="55">
         <v>18</v>
       </c>
-      <c r="C40" s="75"/>
+      <c r="C40" s="55"/>
       <c r="D40" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="E40" s="79">
+      <c r="E40" s="56">
         <v>12</v>
       </c>
       <c r="F40" s="5" t="s">
@@ -5341,12 +5341,12 @@
     </row>
     <row r="41" spans="1:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="72"/>
-      <c r="B41" s="80"/>
-      <c r="C41" s="80"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="81"/>
+      <c r="E41" s="59"/>
       <c r="F41" s="9" t="s">
         <v>52</v>
       </c>
@@ -5361,14 +5361,14 @@
       <c r="A42" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="B42" s="90">
+      <c r="B42" s="66">
         <v>19</v>
       </c>
-      <c r="C42" s="82"/>
+      <c r="C42" s="64"/>
       <c r="D42" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="E42" s="83">
+      <c r="E42" s="65">
         <v>12</v>
       </c>
       <c r="F42" s="2" t="s">
@@ -5383,12 +5383,12 @@
     </row>
     <row r="43" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="71"/>
-      <c r="B43" s="88"/>
-      <c r="C43" s="75"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="55"/>
       <c r="D43" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="E43" s="79"/>
+      <c r="E43" s="56"/>
       <c r="F43" s="5" t="s">
         <v>186</v>
       </c>
@@ -5400,17 +5400,17 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="68" t="s">
+      <c r="A44" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="75">
+      <c r="B44" s="55">
         <v>1</v>
       </c>
-      <c r="C44" s="75"/>
+      <c r="C44" s="55"/>
       <c r="D44" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="E44" s="79">
+      <c r="E44" s="56">
         <v>15</v>
       </c>
       <c r="F44" s="4" t="s">
@@ -5424,13 +5424,13 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="68"/>
-      <c r="B45" s="75"/>
-      <c r="C45" s="75"/>
+      <c r="A45" s="74"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
       <c r="D45" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="79"/>
+      <c r="E45" s="56"/>
       <c r="F45" s="5" t="s">
         <v>189</v>
       </c>
@@ -5442,17 +5442,17 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="68" t="s">
+      <c r="A46" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="75">
+      <c r="B46" s="55">
         <v>2</v>
       </c>
-      <c r="C46" s="75"/>
+      <c r="C46" s="55"/>
       <c r="D46" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="E46" s="79">
+      <c r="E46" s="56">
         <v>18</v>
       </c>
       <c r="F46" s="5" t="s">
@@ -5466,13 +5466,13 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="68"/>
-      <c r="B47" s="75"/>
-      <c r="C47" s="75"/>
+      <c r="A47" s="74"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
       <c r="D47" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E47" s="79"/>
+      <c r="E47" s="56"/>
       <c r="F47" s="5" t="s">
         <v>191</v>
       </c>
@@ -5484,17 +5484,17 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="68" t="s">
+      <c r="A48" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B48" s="88">
+      <c r="B48" s="54">
         <v>3</v>
       </c>
-      <c r="C48" s="75"/>
+      <c r="C48" s="55"/>
       <c r="D48" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="E48" s="79">
+      <c r="E48" s="56">
         <v>15</v>
       </c>
       <c r="F48" s="5" t="s">
@@ -5508,13 +5508,13 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="68"/>
-      <c r="B49" s="88"/>
-      <c r="C49" s="75"/>
+      <c r="A49" s="74"/>
+      <c r="B49" s="54"/>
+      <c r="C49" s="55"/>
       <c r="D49" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="E49" s="79"/>
+      <c r="E49" s="56"/>
       <c r="F49" s="5" t="s">
         <v>193</v>
       </c>
@@ -5526,17 +5526,17 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="68" t="s">
+      <c r="A50" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="88">
+      <c r="B50" s="54">
         <v>4</v>
       </c>
-      <c r="C50" s="75"/>
+      <c r="C50" s="55"/>
       <c r="D50" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="E50" s="79">
+      <c r="E50" s="56">
         <v>18</v>
       </c>
       <c r="F50" s="5" t="s">
@@ -5550,13 +5550,13 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="68"/>
-      <c r="B51" s="88"/>
-      <c r="C51" s="75"/>
+      <c r="A51" s="74"/>
+      <c r="B51" s="54"/>
+      <c r="C51" s="55"/>
       <c r="D51" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="79"/>
+      <c r="E51" s="56"/>
       <c r="F51" s="5" t="s">
         <v>195</v>
       </c>
@@ -5568,17 +5568,17 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="68" t="s">
+      <c r="A52" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B52" s="88">
+      <c r="B52" s="54">
         <v>5</v>
       </c>
-      <c r="C52" s="75"/>
+      <c r="C52" s="55"/>
       <c r="D52" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E52" s="79">
+      <c r="E52" s="56">
         <v>15</v>
       </c>
       <c r="F52" s="5" t="s">
@@ -5592,13 +5592,13 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="68"/>
-      <c r="B53" s="88"/>
-      <c r="C53" s="75"/>
+      <c r="A53" s="74"/>
+      <c r="B53" s="54"/>
+      <c r="C53" s="55"/>
       <c r="D53" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E53" s="79"/>
+      <c r="E53" s="56"/>
       <c r="F53" s="3" t="s">
         <v>59</v>
       </c>
@@ -5610,17 +5610,17 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="68" t="s">
+      <c r="A54" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B54" s="88">
+      <c r="B54" s="54">
         <v>6</v>
       </c>
-      <c r="C54" s="75"/>
+      <c r="C54" s="55"/>
       <c r="D54" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E54" s="79">
+      <c r="E54" s="56">
         <v>25</v>
       </c>
       <c r="F54" s="5" t="s">
@@ -5634,13 +5634,13 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="69"/>
-      <c r="B55" s="89"/>
-      <c r="C55" s="80"/>
+      <c r="A55" s="75"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="58"/>
       <c r="D55" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="E55" s="81"/>
+      <c r="E55" s="59"/>
       <c r="F55" s="9" t="s">
         <v>197</v>
       </c>
@@ -5652,17 +5652,17 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="70" t="s">
+      <c r="A56" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="82">
+      <c r="B56" s="64">
         <v>7</v>
       </c>
-      <c r="C56" s="82"/>
+      <c r="C56" s="64"/>
       <c r="D56" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="E56" s="84"/>
+      <c r="E56" s="67"/>
       <c r="F56" s="33"/>
       <c r="G56" s="2" t="s">
         <v>27</v>
@@ -5672,13 +5672,13 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="68"/>
-      <c r="B57" s="75"/>
-      <c r="C57" s="75"/>
+      <c r="A57" s="74"/>
+      <c r="B57" s="55"/>
+      <c r="C57" s="55"/>
       <c r="D57" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="E57" s="76"/>
+      <c r="E57" s="63"/>
       <c r="F57" s="31"/>
       <c r="G57" s="5" t="s">
         <v>26</v>
@@ -5688,17 +5688,17 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="68" t="s">
+      <c r="A58" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B58" s="75">
+      <c r="B58" s="55">
         <v>8</v>
       </c>
-      <c r="C58" s="75"/>
+      <c r="C58" s="55"/>
       <c r="D58" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="E58" s="79">
+      <c r="E58" s="56">
         <v>28</v>
       </c>
       <c r="F58" s="5" t="s">
@@ -5712,13 +5712,13 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="68"/>
-      <c r="B59" s="75"/>
-      <c r="C59" s="75"/>
+      <c r="A59" s="74"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="55"/>
       <c r="D59" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="E59" s="79"/>
+      <c r="E59" s="56"/>
       <c r="F59" s="5" t="s">
         <v>199</v>
       </c>
@@ -5730,17 +5730,17 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="68" t="s">
+      <c r="A60" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="75">
+      <c r="B60" s="55">
         <v>9</v>
       </c>
-      <c r="C60" s="75"/>
+      <c r="C60" s="55"/>
       <c r="D60" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="E60" s="79">
+      <c r="E60" s="56">
         <v>25</v>
       </c>
       <c r="F60" s="5" t="s">
@@ -5754,13 +5754,13 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="68"/>
-      <c r="B61" s="75"/>
-      <c r="C61" s="75"/>
+      <c r="A61" s="74"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="55"/>
       <c r="D61" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="E61" s="79"/>
+      <c r="E61" s="56"/>
       <c r="F61" s="5" t="s">
         <v>201</v>
       </c>
@@ -5772,17 +5772,17 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="68" t="s">
+      <c r="A62" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B62" s="75">
+      <c r="B62" s="55">
         <v>10</v>
       </c>
-      <c r="C62" s="75"/>
+      <c r="C62" s="55"/>
       <c r="D62" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="E62" s="79">
+      <c r="E62" s="56">
         <v>20</v>
       </c>
       <c r="F62" s="5" t="s">
@@ -5796,13 +5796,13 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="68"/>
-      <c r="B63" s="75"/>
-      <c r="C63" s="75"/>
+      <c r="A63" s="74"/>
+      <c r="B63" s="55"/>
+      <c r="C63" s="55"/>
       <c r="D63" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="E63" s="79"/>
+      <c r="E63" s="56"/>
       <c r="F63" s="5" t="s">
         <v>36</v>
       </c>
@@ -5814,17 +5814,17 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="68" t="s">
+      <c r="A64" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="75">
+      <c r="B64" s="55">
         <v>11</v>
       </c>
-      <c r="C64" s="75"/>
+      <c r="C64" s="55"/>
       <c r="D64" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E64" s="79">
+      <c r="E64" s="56">
         <v>18</v>
       </c>
       <c r="F64" s="5" t="s">
@@ -5838,13 +5838,13 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="68"/>
-      <c r="B65" s="75"/>
-      <c r="C65" s="75"/>
+      <c r="A65" s="74"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="55"/>
       <c r="D65" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E65" s="79"/>
+      <c r="E65" s="56"/>
       <c r="F65" s="5" t="s">
         <v>67</v>
       </c>
@@ -5856,17 +5856,17 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="68" t="s">
+      <c r="A66" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="75">
+      <c r="B66" s="55">
         <v>12</v>
       </c>
-      <c r="C66" s="75"/>
+      <c r="C66" s="55"/>
       <c r="D66" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="E66" s="79">
+      <c r="E66" s="56">
         <v>15</v>
       </c>
       <c r="F66" s="5" t="s">
@@ -5880,13 +5880,13 @@
       </c>
     </row>
     <row r="67" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="68"/>
-      <c r="B67" s="75"/>
-      <c r="C67" s="75"/>
+      <c r="A67" s="74"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="55"/>
       <c r="D67" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="E67" s="79"/>
+      <c r="E67" s="56"/>
       <c r="F67" s="5" t="s">
         <v>202</v>
       </c>
@@ -5898,17 +5898,17 @@
       </c>
     </row>
     <row r="68" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="68" t="s">
+      <c r="A68" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B68" s="75">
+      <c r="B68" s="55">
         <v>13</v>
       </c>
-      <c r="C68" s="75"/>
+      <c r="C68" s="55"/>
       <c r="D68" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="E68" s="79">
+      <c r="E68" s="56">
         <v>15</v>
       </c>
       <c r="F68" s="5" t="s">
@@ -5922,13 +5922,13 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="69"/>
-      <c r="B69" s="80"/>
-      <c r="C69" s="80"/>
+      <c r="A69" s="75"/>
+      <c r="B69" s="58"/>
+      <c r="C69" s="58"/>
       <c r="D69" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="E69" s="81"/>
+      <c r="E69" s="59"/>
       <c r="F69" s="9" t="s">
         <v>205</v>
       </c>
@@ -5940,17 +5940,17 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="70" t="s">
+      <c r="A70" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="B70" s="82">
+      <c r="B70" s="64">
         <v>14</v>
       </c>
-      <c r="C70" s="82"/>
+      <c r="C70" s="64"/>
       <c r="D70" s="33" t="s">
         <v>154</v>
       </c>
-      <c r="E70" s="83">
+      <c r="E70" s="65">
         <v>15</v>
       </c>
       <c r="F70" s="2" t="s">
@@ -5964,13 +5964,13 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="68"/>
-      <c r="B71" s="75"/>
-      <c r="C71" s="75"/>
+      <c r="A71" s="74"/>
+      <c r="B71" s="55"/>
+      <c r="C71" s="55"/>
       <c r="D71" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="E71" s="79"/>
+      <c r="E71" s="56"/>
       <c r="F71" s="5" t="s">
         <v>63</v>
       </c>
@@ -5982,17 +5982,17 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="68" t="s">
+      <c r="A72" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="75">
+      <c r="B72" s="55">
         <v>15</v>
       </c>
-      <c r="C72" s="75"/>
+      <c r="C72" s="55"/>
       <c r="D72" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E72" s="79">
+      <c r="E72" s="56">
         <v>15</v>
       </c>
       <c r="F72" s="5" t="s">
@@ -6006,13 +6006,13 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="68"/>
-      <c r="B73" s="75"/>
-      <c r="C73" s="75"/>
+      <c r="A73" s="74"/>
+      <c r="B73" s="55"/>
+      <c r="C73" s="55"/>
       <c r="D73" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="E73" s="79"/>
+      <c r="E73" s="56"/>
       <c r="F73" s="5" t="s">
         <v>43</v>
       </c>
@@ -6024,17 +6024,17 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="68" t="s">
+      <c r="A74" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="75">
+      <c r="B74" s="55">
         <v>16</v>
       </c>
-      <c r="C74" s="75"/>
+      <c r="C74" s="55"/>
       <c r="D74" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="E74" s="79">
+      <c r="E74" s="56">
         <v>18</v>
       </c>
       <c r="F74" s="5" t="s">
@@ -6048,13 +6048,13 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="68"/>
-      <c r="B75" s="75"/>
-      <c r="C75" s="75"/>
+      <c r="A75" s="74"/>
+      <c r="B75" s="55"/>
+      <c r="C75" s="55"/>
       <c r="D75" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="E75" s="79"/>
+      <c r="E75" s="56"/>
       <c r="F75" s="5" t="s">
         <v>207</v>
       </c>
@@ -6066,17 +6066,17 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="68" t="s">
+      <c r="A76" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B76" s="75">
+      <c r="B76" s="55">
         <v>17</v>
       </c>
-      <c r="C76" s="75"/>
+      <c r="C76" s="55"/>
       <c r="D76" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="E76" s="79">
+      <c r="E76" s="56">
         <v>25</v>
       </c>
       <c r="F76" s="5" t="s">
@@ -6090,13 +6090,13 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="68"/>
-      <c r="B77" s="75"/>
-      <c r="C77" s="75"/>
+      <c r="A77" s="74"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="55"/>
       <c r="D77" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="E77" s="79"/>
+      <c r="E77" s="56"/>
       <c r="F77" s="5" t="s">
         <v>205</v>
       </c>
@@ -6108,17 +6108,17 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="68" t="s">
+      <c r="A78" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="75">
+      <c r="B78" s="55">
         <v>18</v>
       </c>
-      <c r="C78" s="75"/>
+      <c r="C78" s="55"/>
       <c r="D78" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="E78" s="79">
+      <c r="E78" s="56">
         <v>25</v>
       </c>
       <c r="F78" s="5" t="s">
@@ -6132,13 +6132,13 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="68"/>
-      <c r="B79" s="75"/>
-      <c r="C79" s="75"/>
+      <c r="A79" s="74"/>
+      <c r="B79" s="55"/>
+      <c r="C79" s="55"/>
       <c r="D79" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E79" s="79"/>
+      <c r="E79" s="56"/>
       <c r="F79" s="5" t="s">
         <v>209</v>
       </c>
@@ -6150,17 +6150,17 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="68" t="s">
+      <c r="A80" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B80" s="75">
+      <c r="B80" s="55">
         <v>19</v>
       </c>
-      <c r="C80" s="75"/>
+      <c r="C80" s="55"/>
       <c r="D80" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="E80" s="79">
+      <c r="E80" s="56">
         <v>25</v>
       </c>
       <c r="F80" s="5" t="s">
@@ -6174,13 +6174,13 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="68"/>
-      <c r="B81" s="75"/>
-      <c r="C81" s="75"/>
+      <c r="A81" s="74"/>
+      <c r="B81" s="55"/>
+      <c r="C81" s="55"/>
       <c r="D81" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="E81" s="79"/>
+      <c r="E81" s="56"/>
       <c r="F81" s="5" t="s">
         <v>211</v>
       </c>
@@ -6192,17 +6192,17 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="68" t="s">
+      <c r="A82" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B82" s="75">
+      <c r="B82" s="55">
         <v>20</v>
       </c>
-      <c r="C82" s="75"/>
+      <c r="C82" s="55"/>
       <c r="D82" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="E82" s="79">
+      <c r="E82" s="56">
         <v>25</v>
       </c>
       <c r="F82" s="5" t="s">
@@ -6216,13 +6216,13 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="38.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="69"/>
-      <c r="B83" s="80"/>
-      <c r="C83" s="80"/>
+      <c r="A83" s="75"/>
+      <c r="B83" s="58"/>
+      <c r="C83" s="58"/>
       <c r="D83" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="E83" s="81"/>
+      <c r="E83" s="59"/>
       <c r="F83" s="9" t="s">
         <v>213</v>
       </c>
@@ -6234,17 +6234,17 @@
       </c>
     </row>
     <row r="84" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="70" t="s">
+      <c r="A84" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="B84" s="82">
+      <c r="B84" s="64">
         <v>21</v>
       </c>
-      <c r="C84" s="82"/>
+      <c r="C84" s="64"/>
       <c r="D84" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="E84" s="83">
+      <c r="E84" s="65">
         <v>25</v>
       </c>
       <c r="F84" s="2" t="s">
@@ -6258,13 +6258,13 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="68"/>
-      <c r="B85" s="75"/>
-      <c r="C85" s="75"/>
+      <c r="A85" s="74"/>
+      <c r="B85" s="55"/>
+      <c r="C85" s="55"/>
       <c r="D85" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="E85" s="79"/>
+      <c r="E85" s="56"/>
       <c r="F85" s="5" t="s">
         <v>28</v>
       </c>
@@ -6276,17 +6276,17 @@
       </c>
     </row>
     <row r="86" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="68" t="s">
+      <c r="A86" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B86" s="75">
+      <c r="B86" s="55">
         <v>22</v>
       </c>
-      <c r="C86" s="75"/>
+      <c r="C86" s="55"/>
       <c r="D86" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E86" s="79">
+      <c r="E86" s="56">
         <v>15</v>
       </c>
       <c r="F86" s="5" t="s">
@@ -6300,13 +6300,13 @@
       </c>
     </row>
     <row r="87" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="68"/>
-      <c r="B87" s="75"/>
-      <c r="C87" s="75"/>
+      <c r="A87" s="74"/>
+      <c r="B87" s="55"/>
+      <c r="C87" s="55"/>
       <c r="D87" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="79"/>
+      <c r="E87" s="56"/>
       <c r="F87" s="5" t="s">
         <v>215</v>
       </c>
@@ -6318,17 +6318,17 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="68" t="s">
+      <c r="A88" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B88" s="88">
+      <c r="B88" s="54">
         <v>23</v>
       </c>
-      <c r="C88" s="75"/>
+      <c r="C88" s="55"/>
       <c r="D88" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="E88" s="76"/>
+      <c r="E88" s="63"/>
       <c r="F88" s="5" t="s">
         <v>33</v>
       </c>
@@ -6340,13 +6340,13 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="68"/>
-      <c r="B89" s="88"/>
-      <c r="C89" s="75"/>
+      <c r="A89" s="74"/>
+      <c r="B89" s="54"/>
+      <c r="C89" s="55"/>
       <c r="D89" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="E89" s="76"/>
+      <c r="E89" s="63"/>
       <c r="F89" s="5" t="s">
         <v>34</v>
       </c>
@@ -6358,17 +6358,17 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="68" t="s">
+      <c r="A90" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B90" s="75">
+      <c r="B90" s="55">
         <v>24</v>
       </c>
-      <c r="C90" s="75"/>
+      <c r="C90" s="55"/>
       <c r="D90" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="E90" s="76"/>
+      <c r="E90" s="63"/>
       <c r="F90" s="31"/>
       <c r="G90" s="5" t="s">
         <v>27</v>
@@ -6378,13 +6378,13 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="68"/>
-      <c r="B91" s="75"/>
-      <c r="C91" s="75"/>
+      <c r="A91" s="74"/>
+      <c r="B91" s="55"/>
+      <c r="C91" s="55"/>
       <c r="D91" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="E91" s="76"/>
+      <c r="E91" s="63"/>
       <c r="F91" s="31"/>
       <c r="G91" s="5" t="s">
         <v>26</v>
@@ -6394,17 +6394,17 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="68" t="s">
+      <c r="A92" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B92" s="75">
+      <c r="B92" s="55">
         <v>25</v>
       </c>
-      <c r="C92" s="75"/>
+      <c r="C92" s="55"/>
       <c r="D92" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="E92" s="76"/>
+      <c r="E92" s="63"/>
       <c r="F92" s="5" t="s">
         <v>216</v>
       </c>
@@ -6416,13 +6416,13 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="68"/>
-      <c r="B93" s="75"/>
-      <c r="C93" s="75"/>
+      <c r="A93" s="74"/>
+      <c r="B93" s="55"/>
+      <c r="C93" s="55"/>
       <c r="D93" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="E93" s="76"/>
+      <c r="E93" s="63"/>
       <c r="F93" s="5" t="s">
         <v>217</v>
       </c>
@@ -6434,17 +6434,17 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="68" t="s">
+      <c r="A94" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="B94" s="75">
+      <c r="B94" s="55">
         <v>26</v>
       </c>
-      <c r="C94" s="75"/>
+      <c r="C94" s="55"/>
       <c r="D94" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E94" s="76"/>
+      <c r="E94" s="63"/>
       <c r="F94" s="1" t="s">
         <v>44</v>
       </c>
@@ -6456,13 +6456,13 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="68"/>
-      <c r="B95" s="75"/>
-      <c r="C95" s="75"/>
+      <c r="A95" s="74"/>
+      <c r="B95" s="55"/>
+      <c r="C95" s="55"/>
       <c r="D95" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E95" s="76"/>
+      <c r="E95" s="63"/>
       <c r="F95" s="1" t="s">
         <v>45</v>
       </c>
@@ -6474,17 +6474,17 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="58" t="s">
+      <c r="A96" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="B96" s="75">
+      <c r="B96" s="55">
         <v>27</v>
       </c>
-      <c r="C96" s="75"/>
+      <c r="C96" s="55"/>
       <c r="D96" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="E96" s="76"/>
+      <c r="E96" s="63"/>
       <c r="F96" s="31"/>
       <c r="G96" s="5" t="s">
         <v>27</v>
@@ -6494,13 +6494,13 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="58"/>
-      <c r="B97" s="75"/>
-      <c r="C97" s="75"/>
+      <c r="A97" s="81"/>
+      <c r="B97" s="55"/>
+      <c r="C97" s="55"/>
       <c r="D97" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="E97" s="76"/>
+      <c r="E97" s="63"/>
       <c r="F97" s="31"/>
       <c r="G97" s="5" t="s">
         <v>26</v>
@@ -6510,17 +6510,17 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="58" t="s">
+      <c r="A98" s="81" t="s">
         <v>78</v>
       </c>
-      <c r="B98" s="75">
+      <c r="B98" s="55">
         <v>28</v>
       </c>
-      <c r="C98" s="75"/>
+      <c r="C98" s="55"/>
       <c r="D98" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="E98" s="76"/>
+      <c r="E98" s="63"/>
       <c r="F98" s="31"/>
       <c r="G98" s="5" t="s">
         <v>27</v>
@@ -6530,13 +6530,13 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="58"/>
-      <c r="B99" s="75"/>
-      <c r="C99" s="75"/>
+      <c r="A99" s="81"/>
+      <c r="B99" s="55"/>
+      <c r="C99" s="55"/>
       <c r="D99" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="E99" s="76"/>
+      <c r="E99" s="63"/>
       <c r="F99" s="31"/>
       <c r="G99" s="5" t="s">
         <v>26</v>
@@ -6546,14 +6546,14 @@
       </c>
     </row>
     <row r="100" spans="1:8" s="19" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B100" s="77"/>
-      <c r="C100" s="77"/>
-      <c r="E100" s="78"/>
+      <c r="B100" s="68"/>
+      <c r="C100" s="68"/>
+      <c r="E100" s="69"/>
     </row>
     <row r="101" spans="1:8" s="19" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="77"/>
-      <c r="C101" s="77"/>
-      <c r="E101" s="78"/>
+      <c r="B101" s="68"/>
+      <c r="C101" s="68"/>
+      <c r="E101" s="69"/>
     </row>
     <row r="102" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="103" spans="1:8" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6619,181 +6619,6 @@
     <row r="163" ht="38.1" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="199">
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="E48:E49"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="E82:E83"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="C78:C79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="B92:B93"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="E92:E93"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="E94:E95"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="E96:E97"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="A60:A61"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="A98:A99"/>
@@ -6818,6 +6643,181 @@
     <mergeCell ref="A62:A63"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="C94:C95"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="C96:C97"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="B92:B93"/>
+    <mergeCell ref="C92:C93"/>
+    <mergeCell ref="E92:E93"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="C88:C89"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="E82:E83"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="C78:C79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <pageMargins left="0.17" right="0.17" top="0.17" bottom="0.17" header="0.17" footer="0.17"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -6829,8 +6829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6841,10 +6841,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="87"/>
+      <c r="B1" s="91"/>
     </row>
     <row r="2" spans="1:2" ht="35.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -6891,7 +6891,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -6909,19 +6909,19 @@
     <row r="10" spans="1:2" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="52"/>
       <c r="B10" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="52"/>
       <c r="B11" s="48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="53"/>
       <c r="B12" s="50" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>